<commit_message>
atempting to add login
</commit_message>
<xml_diff>
--- a/data/student_labour_report.xlsx
+++ b/data/student_labour_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\savio\PycharmProjects\UscFactDash\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\savio\PycharmProjects\uscIRdash2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4795108A-375C-450E-A686-51103FFE2E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B8290D-4E9E-4A20-AD9F-6FF910E1F355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment" sheetId="1" r:id="rId1"/>
@@ -252,7 +252,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,6 +346,12 @@
       <color rgb="FFFFC000"/>
       <name val="Candara"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1324,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1497D55-6C32-4ECA-8B2C-4BF32BE93E9A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,7 +1352,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>48</v>
       </c>
@@ -1357,7 +1363,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
@@ -1368,7 +1374,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
@@ -1380,6 +1386,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1439,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C69C83F2-7B97-4982-95B4-DCFF0AA58A5A}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>